<commit_message>
update bang phan cong TrThinh
</commit_message>
<xml_diff>
--- a/Bangphancong.xlsx
+++ b/Bangphancong.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tran Lam Khanh Tuong\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TruongThinh\Desktop\QL nhân sự tính lương\QuanLiNhanSuTinhLuong\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFF6208C-2399-486D-AE25-652A4C9502CA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="5760" xr2:uid="{6DDF2BCA-119D-48EF-9070-FB68A0188770}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15348" windowHeight="5760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Tên</t>
   </si>
@@ -40,17 +39,20 @@
   </si>
   <si>
     <t>Trần Lâm Khánh Tường</t>
+  </si>
+  <si>
+    <t>Nguyễn Trường Thịnh</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -82,7 +84,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -393,16 +395,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B80C42DE-2CA7-4134-9914-59A940586247}">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21.69921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -445,6 +447,14 @@
         <v>4</v>
       </c>
     </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>15520844</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A2:A3"/>

</xml_diff>